<commit_message>
TermBO fertig -> fertig für Tests schreiben
</commit_message>
<xml_diff>
--- a/LexikonMvpSoftwareDB/DAO_BO.xlsx
+++ b/LexikonMvpSoftwareDB/DAO_BO.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matti\workspace\LexikonMVP\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19650" windowHeight="7095"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
   <si>
     <t>Sprache vorhanden?</t>
   </si>
@@ -141,6 +137,33 @@
   </si>
   <si>
     <t>Specialty getTechnicalTermList</t>
+  </si>
+  <si>
+    <t>wenn Sprache dargestellt wird, kann es sein, dass es entweder keine Specialty oder TechnicalTerm gibt (in einer Sprache), aber in einer anderen Sprache wurde die Beziehung schon definiert</t>
+  </si>
+  <si>
+    <t>Fragen:</t>
+  </si>
+  <si>
+    <t>Warum gibt es laut den SQL Befehlen beim Aufbau der Tabellen und Beziehungen keine Verbindung zwischen Term und Translation?</t>
+  </si>
+  <si>
+    <t>Befehle werden nicht weiterausgeführt bei TermDAOTest, hängt das mit detach zusammen bzw braucht es hierher ein Merge warum reicht keine neue Transaction?</t>
+  </si>
+  <si>
+    <t>Wenn zB ein Term gelöscht wird, wird automatisch auch der Cascade Rest gelöscht (Translation)?</t>
+  </si>
+  <si>
+    <t>Fremdschlüsselbeziehung wird bei POJO als Objekt angegeben (zB bei Translation -&gt; Language, Term) aber als ID des Objekts gespeichert: wie ist der Zugriff bei einer SQL Abfrage -&gt; zB man will alle Translations einer Specialty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bedingung: </t>
+  </si>
+  <si>
+    <t>specialty darf niemals den gleichen "name" wie technicalTerm haben</t>
+  </si>
+  <si>
+    <t>gleiche namen bei unterschiedlichen translation/sprachen sind möglich</t>
   </si>
 </sst>
 </file>
@@ -473,20 +496,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G75"/>
+  <dimension ref="B3:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.75" customWidth="1"/>
-    <col min="3" max="3" width="27.125" customWidth="1"/>
-    <col min="4" max="4" width="23.625" customWidth="1"/>
-    <col min="5" max="5" width="20.75" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.375" customWidth="1"/>
-    <col min="7" max="7" width="21.125" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -828,14 +851,14 @@
       <c r="D64" s="1"/>
       <c r="F64" s="1"/>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D65" s="1"/>
       <c r="E65" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F65" s="1"/>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D66" s="1" t="s">
         <v>1</v>
       </c>
@@ -843,7 +866,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D67" s="1" t="s">
         <v>19</v>
       </c>
@@ -851,18 +874,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D68" s="1"/>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D69" s="1"/>
       <c r="E69" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F69" s="1"/>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>29</v>
       </c>
@@ -873,7 +896,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
         <v>31</v>
       </c>
@@ -881,7 +904,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>34</v>
       </c>
@@ -892,13 +915,70 @@
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
         <v>36</v>
       </c>
       <c r="D75" t="s">
         <v>38</v>
       </c>
+    </row>
+    <row r="77" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>39</v>
+      </c>
+      <c r="E77" s="1"/>
+    </row>
+    <row r="78" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>45</v>
+      </c>
+      <c r="C78" t="s">
+        <v>46</v>
+      </c>
+      <c r="E78" s="1"/>
+    </row>
+    <row r="79" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>47</v>
+      </c>
+      <c r="E79" s="1"/>
+    </row>
+    <row r="80" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E80" s="1"/>
+    </row>
+    <row r="81" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E81" s="1"/>
+    </row>
+    <row r="82" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E82" s="1"/>
+    </row>
+    <row r="83" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>40</v>
+      </c>
+      <c r="C83" t="s">
+        <v>41</v>
+      </c>
+      <c r="E83" s="1"/>
+    </row>
+    <row r="84" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>42</v>
+      </c>
+      <c r="E84" s="1"/>
+    </row>
+    <row r="85" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>43</v>
+      </c>
+      <c r="E85" s="1"/>
+    </row>
+    <row r="86" spans="2:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>44</v>
+      </c>
+      <c r="E86" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>